<commit_message>
add Material class and basic functions
</commit_message>
<xml_diff>
--- a/sanitation/data/lca_data/materials.xlsx
+++ b/sanitation/data/lca_data/materials.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/sanitation_Yalin/sanitation/data/lca_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FBA20838-FC4C-704A-8717-594EA19578B7}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{935E0A0B-8DD3-6742-99D3-41177F9390EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{334ECFB3-DEC2-8F4C-BB9E-2452E2730A3A}"/>
   <bookViews>
     <workbookView xWindow="5980" yWindow="2860" windowWidth="27240" windowHeight="16440" xr2:uid="{BD97E243-0BB4-3F42-9EBC-00D49E7EE019}"/>
   </bookViews>
   <sheets>
-    <sheet name="GHG" sheetId="1" r:id="rId1"/>
+    <sheet name="GWP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,15 +42,9 @@
     <t>uniform</t>
   </si>
   <si>
-    <t>kg CO2eq/m3</t>
-  </si>
-  <si>
     <t>Wood</t>
   </si>
   <si>
-    <t>kg CO2eq/kg</t>
-  </si>
-  <si>
     <t>Bricks</t>
   </si>
   <si>
@@ -69,12 +63,6 @@
     <t>Excavation</t>
   </si>
   <si>
-    <t>Stainless steel sheet</t>
-  </si>
-  <si>
-    <t>Stainless steel</t>
-  </si>
-  <si>
     <t>Steel</t>
   </si>
   <si>
@@ -93,10 +81,22 @@
     <t>expected</t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
     <t>material</t>
+  </si>
+  <si>
+    <t>functional_unit</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>StainlessSteel</t>
+  </si>
+  <si>
+    <t>StainlessSteelSheet</t>
   </si>
 </sst>
 </file>
@@ -159,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -168,6 +168,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +487,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,41 +498,41 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4">
+        <v>17</v>
+      </c>
+      <c r="C2" s="6">
         <v>2.5499999999999998</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="6">
         <v>2.13</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="6">
         <v>3.15</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -542,18 +544,18 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6">
         <v>4.33</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="6">
         <v>3.07</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="6">
         <v>5.5</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -565,18 +567,18 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6">
         <v>0.65</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="6">
         <v>0.71</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -588,18 +590,18 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6">
         <v>0.53</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="6">
         <v>0.51</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="6">
         <v>0.55000000000000004</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -611,18 +613,18 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
         <v>1.97</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="6">
         <v>1.93</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="6">
         <v>2.0099999999999998</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -634,18 +636,18 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="6">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -657,18 +659,18 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4">
+        <v>17</v>
+      </c>
+      <c r="C8" s="6">
         <v>1.2E-2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="6">
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -680,18 +682,18 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7">
         <v>1.08</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="7">
         <v>0.97</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="7">
         <v>1.19</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -703,18 +705,18 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3">
+        <v>17</v>
+      </c>
+      <c r="C10" s="7">
         <v>0.28000000000000003</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="7">
         <v>0.25</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="7">
         <v>0.31</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -726,18 +728,18 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="4">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6">
         <v>197</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="6">
         <v>186</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="6">
         <v>208</v>
       </c>
       <c r="F11" s="3" t="s">

</xml_diff>